<commit_message>
update notes through 2.1
</commit_message>
<xml_diff>
--- a/Stat5100/course/S20 Schedule (Stat 5100).xlsx
+++ b/Stat5100/course/S20 Schedule (Stat 5100).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3332A88D-80F2-4EAB-9EFA-77E416C46DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E412692-B4BE-4248-B454-0C106B273839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,18 +133,6 @@
     <t>Mythos of Model Interpretability*</t>
   </si>
   <si>
-    <t xml:space="preserve">(3/31) Quiz 4 </t>
-  </si>
-  <si>
-    <t>(4/14) Quiz 5</t>
-  </si>
-  <si>
-    <t>(2/18) Quiz 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2/4) Quiz 1 </t>
-  </si>
-  <si>
     <t>1.4: Data Exploration</t>
   </si>
   <si>
@@ -178,9 +166,6 @@
     <t>Project 2 Papers - First Draft</t>
   </si>
   <si>
-    <t>(3/17) Quiz 3</t>
-  </si>
-  <si>
     <t>No Class - Required Group Meetings with Instructor</t>
   </si>
   <si>
@@ -260,6 +245,21 @@
   </si>
   <si>
     <t>Final Project Slides - Final Draft (pdf format)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 1 </t>
+  </si>
+  <si>
+    <t>Quiz 2</t>
+  </si>
+  <si>
+    <t>Quiz 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 4 </t>
+  </si>
+  <si>
+    <t>Quiz 5</t>
   </si>
 </sst>
 </file>
@@ -688,26 +688,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" customWidth="1"/>
-    <col min="4" max="4" width="24.796875" customWidth="1"/>
+    <col min="3" max="3" width="50.36328125" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -718,7 +718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>43836</v>
       </c>
@@ -727,7 +727,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43838</v>
       </c>
@@ -736,47 +736,47 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>43840</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>43843</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>43845</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>43847</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>43850</v>
       </c>
@@ -785,16 +785,16 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>43852</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>43854</v>
       </c>
@@ -803,25 +803,25 @@
       </c>
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>43857</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>43859</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>43861</v>
       </c>
@@ -832,27 +832,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>43864</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>43866</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>43868</v>
       </c>
@@ -860,28 +860,28 @@
         <v>2</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>43871</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>43873</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>43875</v>
       </c>
@@ -889,10 +889,10 @@
         <v>2</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>43878</v>
       </c>
@@ -901,18 +901,18 @@
       </c>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>43880</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>43882</v>
       </c>
@@ -920,10 +920,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>43885</v>
       </c>
@@ -934,16 +934,16 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>43887</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>43889</v>
       </c>
@@ -951,10 +951,10 @@
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>43892</v>
       </c>
@@ -963,7 +963,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>43894</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>412790</v>
       </c>
@@ -981,16 +981,16 @@
       </c>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>43899</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>43901</v>
       </c>
@@ -998,10 +998,10 @@
         <v>2</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>43903</v>
       </c>
@@ -1009,30 +1009,30 @@
         <v>3</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>43906</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>43908</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>43910</v>
       </c>
@@ -1040,10 +1040,10 @@
         <v>2</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>43913</v>
       </c>
@@ -1052,18 +1052,18 @@
       </c>
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>43915</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>43917</v>
       </c>
@@ -1071,39 +1071,39 @@
         <v>3</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>43920</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C39" s="5"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>43922</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>43924</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>43927</v>
       </c>
@@ -1112,16 +1112,16 @@
       </c>
       <c r="C42" s="6"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>43929</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43931</v>
       </c>
@@ -1129,32 +1129,32 @@
         <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>43934</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>43936</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>43938</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="C47" s="10"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>43941</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="C48" s="12"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>43943</v>
       </c>
@@ -1180,31 +1180,31 @@
         <v>7</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>43945</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B52" s="22"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B53" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="22" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notes through module 4
</commit_message>
<xml_diff>
--- a/Stat5100/course/S20 Schedule (Stat 5100).xlsx
+++ b/Stat5100/course/S20 Schedule (Stat 5100).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brennan\github\teaching\Stat5100\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C64497B-769A-4C56-8062-E9E8C852CA7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A40D690-1CB5-41D4-B3F3-CF4BB85B2195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -154,18 +154,9 @@
     <t>Intro to Scientific Writing</t>
   </si>
   <si>
-    <t>Project 2 Papers - Final Draft</t>
-  </si>
-  <si>
-    <t>Project 2 Peer Review</t>
-  </si>
-  <si>
     <t>Project 1 Paper - 1st Draft/HW 3</t>
   </si>
   <si>
-    <t>Project 2 Papers - First Draft</t>
-  </si>
-  <si>
     <t>No Class - Required Group Meetings with Instructor</t>
   </si>
   <si>
@@ -211,9 +202,6 @@
     <t>7.1: Quantile Regression</t>
   </si>
   <si>
-    <t xml:space="preserve">HW 4/Final Project Proposals </t>
-  </si>
-  <si>
     <t xml:space="preserve">HW 6/Final Project Papers - First Draft </t>
   </si>
   <si>
@@ -238,9 +226,6 @@
     <t>Project 1 Paper - Final Draft/Mid-Semester Eval</t>
   </si>
   <si>
-    <t>HW 5</t>
-  </si>
-  <si>
     <t>Final Project Slides - First Draft (pdf format)</t>
   </si>
   <si>
@@ -263,6 +248,18 @@
   </si>
   <si>
     <t>D.2 Group Work Primer (make up)</t>
+  </si>
+  <si>
+    <t>Project 2 Peer Review/Final Project Proposals</t>
+  </si>
+  <si>
+    <t>HW 4/Project 2 Papers - First Draft</t>
+  </si>
+  <si>
+    <t>HW 5/Project 2 Papers - Final Draft</t>
+  </si>
+  <si>
+    <t>No Class</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -409,6 +406,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,7 +742,7 @@
         <v>43840</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>12</v>
@@ -840,7 +838,7 @@
         <v>43864</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5"/>
     </row>
@@ -849,10 +847,10 @@
         <v>43866</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -871,7 +869,7 @@
         <v>43871</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C18" s="11"/>
     </row>
@@ -880,7 +878,7 @@
         <v>43873</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -892,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -909,10 +907,10 @@
         <v>43880</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -923,7 +921,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -942,7 +940,7 @@
         <v>43887</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C25" s="12"/>
     </row>
@@ -954,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -989,7 +987,7 @@
         <v>43899</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C30" s="6"/>
     </row>
@@ -998,11 +996,9 @@
         <v>43901</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>28</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
@@ -1012,15 +1008,15 @@
         <v>3</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>43906</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>48</v>
+      <c r="B33" s="26" t="s">
+        <v>60</v>
       </c>
       <c r="C33" s="5"/>
     </row>
@@ -1029,21 +1025,21 @@
         <v>43908</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>43910</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>2</v>
+      <c r="B35" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1060,11 +1056,9 @@
         <v>43915</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>25</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
@@ -1074,7 +1068,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1082,7 +1076,7 @@
         <v>43920</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C39" s="5"/>
     </row>
@@ -1091,10 +1085,10 @@
         <v>43922</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1102,7 +1096,7 @@
         <v>43924</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C41" s="10"/>
     </row>
@@ -1120,7 +1114,7 @@
         <v>43929</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C43" s="3"/>
     </row>
@@ -1132,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1140,10 +1134,10 @@
         <v>43934</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1151,10 +1145,10 @@
         <v>43936</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1183,7 +1177,7 @@
         <v>7</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1191,10 +1185,10 @@
         <v>43945</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1207,7 +1201,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>